<commit_message>
Base model changed, added some methods to DataBaseHelper
</commit_message>
<xml_diff>
--- a/DjantaBase.xlsx
+++ b/DjantaBase.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Mironov\IT Talents\JantaBG\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{79E8BA9C-7CF4-47E7-B1F3-94ED52E29318}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
     <sheet name="Offer" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>USER</t>
   </si>
@@ -70,12 +70,27 @@
   </si>
   <si>
     <t>OFFER_TABLE</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>REAL</t>
+  </si>
+  <si>
+    <t>NUMERIC</t>
+  </si>
+  <si>
+    <t>INTEGER</t>
+  </si>
+  <si>
+    <t>ID(PK)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -450,27 +465,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{606A2686-2B99-456A-A2DD-BBBB25FE6E7C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.21875" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -485,16 +500,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -503,7 +532,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -512,7 +541,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -521,7 +550,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -530,7 +559,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -539,7 +568,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -548,7 +577,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -557,7 +586,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -566,7 +595,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="E15" s="3" t="s">
         <v>13</v>
       </c>
@@ -583,22 +612,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D73C04-0FBF-4B50-9C8C-E7AE6935F8E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
@@ -615,64 +644,88 @@
       <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-    </row>
-    <row r="15" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="E15" s="3" t="s">
         <v>14</v>
       </c>
@@ -684,5 +737,6 @@
     <mergeCell ref="E15:G15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added toolbar logo and welcome text, added userinfo texts, added add offer texts, start of choose image functionality
</commit_message>
<xml_diff>
--- a/DjantaBase.xlsx
+++ b/DjantaBase.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Mironov\IT Talents\JantaBG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\Git\JantaBG\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -465,19 +465,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -500,7 +500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -523,7 +523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -532,7 +532,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -541,7 +541,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -550,7 +550,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -559,7 +559,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -568,7 +568,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -577,7 +577,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -586,7 +586,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -595,7 +595,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E15" s="3" t="s">
         <v>13</v>
       </c>
@@ -612,20 +612,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -648,7 +648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -671,7 +671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -680,7 +680,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -689,7 +689,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -698,7 +698,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -707,7 +707,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -716,7 +716,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -725,7 +725,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="E15" s="3" t="s">
         <v>14</v>
       </c>

</xml_diff>